<commit_message>
[EPS] BOM fixes and re-export
</commit_message>
<xml_diff>
--- a/flight-BOM_2019-09-19.xlsx
+++ b/flight-BOM_2019-09-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorna.l\pcbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB060744-AF35-4DCA-BA8E-21CD78274A17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426F217-A275-4001-B39D-65CCD47A9399}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pay-ssm" sheetId="1" r:id="rId1"/>
@@ -2920,8 +2920,8 @@
   </sheetPr>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6258,7 +6258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF0471E-BEAB-4D20-8223-518A1B1B1652}">
   <dimension ref="A1:AZ101"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="H54" sqref="H54:N54"/>
     </sheetView>
   </sheetViews>

</xml_diff>